<commit_message>
EcommerceBack - Estructura basica y Template v1
</commit_message>
<xml_diff>
--- a/Documentacion/Cronograma_EcommerceCBD_v02.xlsx
+++ b/Documentacion/Cronograma_EcommerceCBD_v02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oavalos/Documents/Personal/Proyecto CBD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oavalos/Documents/Personal/Proyecto CBD/Codigo/Documentacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34684BD-E518-4945-A6DD-04AC63DAFE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02057902-F9D6-3C40-98DA-0BA869CDA0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRONOGRAMA" sheetId="1" r:id="rId1"/>
@@ -615,7 +615,7 @@
       <name val="Corbel"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,12 +720,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
@@ -740,6 +734,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1164,7 +1170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1521,6 +1527,104 @@
     <xf numFmtId="0" fontId="20" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="48" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1531,109 +1635,20 @@
     <xf numFmtId="0" fontId="48" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="48" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1956,8 +1971,8 @@
   </sheetPr>
   <dimension ref="A1:CK68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2064,27 +2079,27 @@
     </row>
     <row r="2" spans="1:78" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="164" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="128"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="127"/>
-      <c r="S2" s="127"/>
-      <c r="T2" s="127"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="166"/>
+      <c r="N2" s="166"/>
+      <c r="O2" s="166"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
+      <c r="S2" s="165"/>
+      <c r="T2" s="165"/>
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
       <c r="W2" s="10"/>
@@ -2231,54 +2246,54 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="129" t="s">
+      <c r="E4" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="130"/>
-      <c r="G4" s="130"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="18"/>
-      <c r="I4" s="131" t="s">
+      <c r="I4" s="153" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="131"/>
-      <c r="N4" s="131"/>
-      <c r="O4" s="131"/>
-      <c r="P4" s="132"/>
-      <c r="Q4" s="132"/>
-      <c r="R4" s="132"/>
-      <c r="S4" s="132"/>
-      <c r="T4" s="132"/>
-      <c r="U4" s="132"/>
+      <c r="J4" s="153"/>
+      <c r="K4" s="153"/>
+      <c r="L4" s="153"/>
+      <c r="M4" s="153"/>
+      <c r="N4" s="153"/>
+      <c r="O4" s="153"/>
+      <c r="P4" s="154"/>
+      <c r="Q4" s="154"/>
+      <c r="R4" s="154"/>
+      <c r="S4" s="154"/>
+      <c r="T4" s="154"/>
+      <c r="U4" s="154"/>
       <c r="V4" s="64"/>
       <c r="W4" s="64"/>
-      <c r="X4" s="133" t="s">
+      <c r="X4" s="168" t="s">
         <v>100</v>
       </c>
-      <c r="Y4" s="130"/>
-      <c r="Z4" s="130"/>
-      <c r="AA4" s="130"/>
-      <c r="AB4" s="130"/>
-      <c r="AC4" s="130"/>
-      <c r="AD4" s="130"/>
-      <c r="AE4" s="130"/>
-      <c r="AF4" s="130"/>
-      <c r="AG4" s="130"/>
-      <c r="AH4" s="130"/>
-      <c r="AI4" s="130"/>
-      <c r="AJ4" s="130"/>
-      <c r="AK4" s="130"/>
-      <c r="AL4" s="130"/>
-      <c r="AM4" s="130"/>
-      <c r="AN4" s="130"/>
-      <c r="AO4" s="130"/>
-      <c r="AP4" s="130"/>
-      <c r="AQ4" s="130"/>
-      <c r="AR4" s="130"/>
-      <c r="AS4" s="130"/>
-      <c r="AT4" s="130"/>
+      <c r="Y4" s="160"/>
+      <c r="Z4" s="160"/>
+      <c r="AA4" s="160"/>
+      <c r="AB4" s="160"/>
+      <c r="AC4" s="160"/>
+      <c r="AD4" s="160"/>
+      <c r="AE4" s="160"/>
+      <c r="AF4" s="160"/>
+      <c r="AG4" s="160"/>
+      <c r="AH4" s="160"/>
+      <c r="AI4" s="160"/>
+      <c r="AJ4" s="160"/>
+      <c r="AK4" s="160"/>
+      <c r="AL4" s="160"/>
+      <c r="AM4" s="160"/>
+      <c r="AN4" s="160"/>
+      <c r="AO4" s="160"/>
+      <c r="AP4" s="160"/>
+      <c r="AQ4" s="160"/>
+      <c r="AR4" s="160"/>
+      <c r="AS4" s="160"/>
+      <c r="AT4" s="160"/>
       <c r="AU4" s="94"/>
       <c r="AV4" s="94"/>
       <c r="AW4" s="94"/>
@@ -2319,54 +2334,54 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="19"/>
-      <c r="E5" s="139" t="s">
+      <c r="E5" s="159" t="s">
         <v>98</v>
       </c>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
       <c r="H5" s="20"/>
-      <c r="I5" s="131" t="s">
+      <c r="I5" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="131"/>
-      <c r="N5" s="131"/>
-      <c r="O5" s="131"/>
-      <c r="P5" s="132"/>
-      <c r="Q5" s="132"/>
-      <c r="R5" s="132"/>
-      <c r="S5" s="132"/>
-      <c r="T5" s="132"/>
-      <c r="U5" s="132"/>
+      <c r="J5" s="153"/>
+      <c r="K5" s="153"/>
+      <c r="L5" s="153"/>
+      <c r="M5" s="153"/>
+      <c r="N5" s="153"/>
+      <c r="O5" s="153"/>
+      <c r="P5" s="154"/>
+      <c r="Q5" s="154"/>
+      <c r="R5" s="154"/>
+      <c r="S5" s="154"/>
+      <c r="T5" s="154"/>
+      <c r="U5" s="154"/>
       <c r="V5" s="64"/>
       <c r="W5" s="64"/>
-      <c r="X5" s="140" t="s">
+      <c r="X5" s="161" t="s">
         <v>27</v>
       </c>
-      <c r="Y5" s="130"/>
-      <c r="Z5" s="130"/>
-      <c r="AA5" s="130"/>
-      <c r="AB5" s="130"/>
-      <c r="AC5" s="130"/>
-      <c r="AD5" s="130"/>
-      <c r="AE5" s="130"/>
-      <c r="AF5" s="130"/>
-      <c r="AG5" s="130"/>
-      <c r="AH5" s="130"/>
-      <c r="AI5" s="130"/>
-      <c r="AJ5" s="130"/>
-      <c r="AK5" s="130"/>
-      <c r="AL5" s="130"/>
-      <c r="AM5" s="130"/>
-      <c r="AN5" s="130"/>
-      <c r="AO5" s="130"/>
-      <c r="AP5" s="130"/>
-      <c r="AQ5" s="130"/>
-      <c r="AR5" s="130"/>
-      <c r="AS5" s="130"/>
-      <c r="AT5" s="130"/>
+      <c r="Y5" s="160"/>
+      <c r="Z5" s="160"/>
+      <c r="AA5" s="160"/>
+      <c r="AB5" s="160"/>
+      <c r="AC5" s="160"/>
+      <c r="AD5" s="160"/>
+      <c r="AE5" s="160"/>
+      <c r="AF5" s="160"/>
+      <c r="AG5" s="160"/>
+      <c r="AH5" s="160"/>
+      <c r="AI5" s="160"/>
+      <c r="AJ5" s="160"/>
+      <c r="AK5" s="160"/>
+      <c r="AL5" s="160"/>
+      <c r="AM5" s="160"/>
+      <c r="AN5" s="160"/>
+      <c r="AO5" s="160"/>
+      <c r="AP5" s="160"/>
+      <c r="AQ5" s="160"/>
+      <c r="AR5" s="160"/>
+      <c r="AS5" s="160"/>
+      <c r="AT5" s="160"/>
       <c r="AU5" s="94"/>
       <c r="AV5" s="94"/>
       <c r="AW5" s="94"/>
@@ -2573,67 +2588,67 @@
         <v>5</v>
       </c>
       <c r="H8" s="28"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
-      <c r="K8" s="134"/>
-      <c r="L8" s="134"/>
-      <c r="M8" s="134"/>
-      <c r="N8" s="134"/>
-      <c r="O8" s="134"/>
-      <c r="P8" s="135"/>
-      <c r="Q8" s="135"/>
-      <c r="R8" s="135"/>
-      <c r="S8" s="135"/>
-      <c r="T8" s="135"/>
-      <c r="U8" s="135"/>
-      <c r="V8" s="135"/>
-      <c r="W8" s="135"/>
-      <c r="X8" s="135"/>
-      <c r="Y8" s="135"/>
-      <c r="Z8" s="135"/>
-      <c r="AA8" s="136"/>
-      <c r="AB8" s="134"/>
-      <c r="AC8" s="134"/>
-      <c r="AD8" s="134"/>
-      <c r="AE8" s="134"/>
-      <c r="AF8" s="134"/>
-      <c r="AG8" s="134"/>
-      <c r="AH8" s="134"/>
-      <c r="AI8" s="134"/>
-      <c r="AJ8" s="134"/>
-      <c r="AK8" s="134"/>
-      <c r="AL8" s="134"/>
-      <c r="AM8" s="134"/>
-      <c r="AN8" s="134"/>
-      <c r="AO8" s="134"/>
-      <c r="AP8" s="134"/>
-      <c r="AQ8" s="134"/>
-      <c r="AR8" s="134"/>
-      <c r="AS8" s="135"/>
-      <c r="AT8" s="135"/>
-      <c r="AU8" s="136"/>
-      <c r="AV8" s="134"/>
-      <c r="AW8" s="134"/>
-      <c r="AX8" s="134"/>
-      <c r="AY8" s="134"/>
-      <c r="AZ8" s="134"/>
-      <c r="BA8" s="134"/>
-      <c r="BB8" s="134"/>
-      <c r="BC8" s="134"/>
-      <c r="BD8" s="134"/>
-      <c r="BE8" s="134"/>
-      <c r="BF8" s="134"/>
-      <c r="BG8" s="134"/>
-      <c r="BH8" s="134"/>
-      <c r="BI8" s="134"/>
-      <c r="BJ8" s="134"/>
-      <c r="BK8" s="134"/>
-      <c r="BL8" s="134"/>
-      <c r="BM8" s="135"/>
-      <c r="BN8" s="135"/>
-      <c r="BO8" s="135"/>
-      <c r="BP8" s="135"/>
-      <c r="BQ8" s="135"/>
+      <c r="I8" s="155"/>
+      <c r="J8" s="155"/>
+      <c r="K8" s="155"/>
+      <c r="L8" s="155"/>
+      <c r="M8" s="155"/>
+      <c r="N8" s="155"/>
+      <c r="O8" s="155"/>
+      <c r="P8" s="136"/>
+      <c r="Q8" s="136"/>
+      <c r="R8" s="136"/>
+      <c r="S8" s="136"/>
+      <c r="T8" s="136"/>
+      <c r="U8" s="136"/>
+      <c r="V8" s="136"/>
+      <c r="W8" s="136"/>
+      <c r="X8" s="136"/>
+      <c r="Y8" s="136"/>
+      <c r="Z8" s="136"/>
+      <c r="AA8" s="156"/>
+      <c r="AB8" s="155"/>
+      <c r="AC8" s="155"/>
+      <c r="AD8" s="155"/>
+      <c r="AE8" s="155"/>
+      <c r="AF8" s="155"/>
+      <c r="AG8" s="155"/>
+      <c r="AH8" s="155"/>
+      <c r="AI8" s="155"/>
+      <c r="AJ8" s="155"/>
+      <c r="AK8" s="155"/>
+      <c r="AL8" s="155"/>
+      <c r="AM8" s="155"/>
+      <c r="AN8" s="155"/>
+      <c r="AO8" s="155"/>
+      <c r="AP8" s="155"/>
+      <c r="AQ8" s="155"/>
+      <c r="AR8" s="155"/>
+      <c r="AS8" s="136"/>
+      <c r="AT8" s="136"/>
+      <c r="AU8" s="156"/>
+      <c r="AV8" s="155"/>
+      <c r="AW8" s="155"/>
+      <c r="AX8" s="155"/>
+      <c r="AY8" s="155"/>
+      <c r="AZ8" s="155"/>
+      <c r="BA8" s="155"/>
+      <c r="BB8" s="155"/>
+      <c r="BC8" s="155"/>
+      <c r="BD8" s="155"/>
+      <c r="BE8" s="155"/>
+      <c r="BF8" s="155"/>
+      <c r="BG8" s="155"/>
+      <c r="BH8" s="155"/>
+      <c r="BI8" s="155"/>
+      <c r="BJ8" s="155"/>
+      <c r="BK8" s="155"/>
+      <c r="BL8" s="155"/>
+      <c r="BM8" s="136"/>
+      <c r="BN8" s="136"/>
+      <c r="BO8" s="136"/>
+      <c r="BP8" s="136"/>
+      <c r="BQ8" s="136"/>
       <c r="BR8" s="29"/>
       <c r="BS8" s="22"/>
       <c r="BT8" s="22"/>
@@ -2646,87 +2661,87 @@
     </row>
     <row r="9" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="30"/>
-      <c r="B9" s="143"/>
-      <c r="C9" s="144" t="s">
+      <c r="B9" s="150"/>
+      <c r="C9" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="135"/>
-      <c r="E9" s="135"/>
-      <c r="F9" s="135"/>
-      <c r="G9" s="144" t="s">
+      <c r="D9" s="136"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
+      <c r="G9" s="151" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="144" t="s">
+      <c r="H9" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="141" t="s">
+      <c r="I9" s="162" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="141"/>
-      <c r="K9" s="141"/>
-      <c r="L9" s="141"/>
-      <c r="M9" s="141"/>
-      <c r="N9" s="141"/>
-      <c r="O9" s="141"/>
-      <c r="P9" s="135"/>
-      <c r="Q9" s="135"/>
-      <c r="R9" s="135"/>
-      <c r="S9" s="135"/>
-      <c r="T9" s="135"/>
-      <c r="U9" s="135"/>
-      <c r="V9" s="135"/>
-      <c r="W9" s="135"/>
-      <c r="X9" s="135"/>
-      <c r="Y9" s="135"/>
-      <c r="Z9" s="135"/>
-      <c r="AA9" s="142" t="s">
+      <c r="J9" s="162"/>
+      <c r="K9" s="162"/>
+      <c r="L9" s="162"/>
+      <c r="M9" s="162"/>
+      <c r="N9" s="162"/>
+      <c r="O9" s="162"/>
+      <c r="P9" s="136"/>
+      <c r="Q9" s="136"/>
+      <c r="R9" s="136"/>
+      <c r="S9" s="136"/>
+      <c r="T9" s="136"/>
+      <c r="U9" s="136"/>
+      <c r="V9" s="136"/>
+      <c r="W9" s="136"/>
+      <c r="X9" s="136"/>
+      <c r="Y9" s="136"/>
+      <c r="Z9" s="136"/>
+      <c r="AA9" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="AB9" s="142"/>
-      <c r="AC9" s="142"/>
-      <c r="AD9" s="142"/>
-      <c r="AE9" s="142"/>
-      <c r="AF9" s="142"/>
-      <c r="AG9" s="142"/>
-      <c r="AH9" s="142"/>
-      <c r="AI9" s="142"/>
-      <c r="AJ9" s="142"/>
-      <c r="AK9" s="142"/>
-      <c r="AL9" s="142"/>
-      <c r="AM9" s="142"/>
-      <c r="AN9" s="142"/>
-      <c r="AO9" s="142"/>
-      <c r="AP9" s="142"/>
-      <c r="AQ9" s="142"/>
-      <c r="AR9" s="142"/>
-      <c r="AS9" s="135"/>
-      <c r="AT9" s="135"/>
-      <c r="AU9" s="142" t="s">
+      <c r="AB9" s="163"/>
+      <c r="AC9" s="163"/>
+      <c r="AD9" s="163"/>
+      <c r="AE9" s="163"/>
+      <c r="AF9" s="163"/>
+      <c r="AG9" s="163"/>
+      <c r="AH9" s="163"/>
+      <c r="AI9" s="163"/>
+      <c r="AJ9" s="163"/>
+      <c r="AK9" s="163"/>
+      <c r="AL9" s="163"/>
+      <c r="AM9" s="163"/>
+      <c r="AN9" s="163"/>
+      <c r="AO9" s="163"/>
+      <c r="AP9" s="163"/>
+      <c r="AQ9" s="163"/>
+      <c r="AR9" s="163"/>
+      <c r="AS9" s="136"/>
+      <c r="AT9" s="136"/>
+      <c r="AU9" s="163" t="s">
         <v>29</v>
       </c>
-      <c r="AV9" s="142"/>
-      <c r="AW9" s="142"/>
-      <c r="AX9" s="142"/>
-      <c r="AY9" s="142"/>
-      <c r="AZ9" s="142"/>
-      <c r="BA9" s="142"/>
-      <c r="BB9" s="142"/>
-      <c r="BC9" s="142"/>
-      <c r="BD9" s="142"/>
-      <c r="BE9" s="142"/>
-      <c r="BF9" s="142"/>
-      <c r="BG9" s="142"/>
-      <c r="BH9" s="142"/>
-      <c r="BI9" s="142"/>
-      <c r="BJ9" s="142"/>
-      <c r="BK9" s="142"/>
-      <c r="BL9" s="142"/>
-      <c r="BM9" s="135"/>
-      <c r="BN9" s="135"/>
-      <c r="BO9" s="135"/>
-      <c r="BP9" s="135"/>
-      <c r="BQ9" s="135"/>
-      <c r="BR9" s="137"/>
+      <c r="AV9" s="163"/>
+      <c r="AW9" s="163"/>
+      <c r="AX9" s="163"/>
+      <c r="AY9" s="163"/>
+      <c r="AZ9" s="163"/>
+      <c r="BA9" s="163"/>
+      <c r="BB9" s="163"/>
+      <c r="BC9" s="163"/>
+      <c r="BD9" s="163"/>
+      <c r="BE9" s="163"/>
+      <c r="BF9" s="163"/>
+      <c r="BG9" s="163"/>
+      <c r="BH9" s="163"/>
+      <c r="BI9" s="163"/>
+      <c r="BJ9" s="163"/>
+      <c r="BK9" s="163"/>
+      <c r="BL9" s="163"/>
+      <c r="BM9" s="136"/>
+      <c r="BN9" s="136"/>
+      <c r="BO9" s="136"/>
+      <c r="BP9" s="136"/>
+      <c r="BQ9" s="136"/>
+      <c r="BR9" s="157"/>
       <c r="BS9" s="31"/>
       <c r="BT9" s="31"/>
       <c r="BU9" s="31"/>
@@ -2738,50 +2753,50 @@
     </row>
     <row r="10" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32"/>
-      <c r="B10" s="135"/>
-      <c r="C10" s="135"/>
-      <c r="D10" s="135"/>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="33">
+      <c r="B10" s="136"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="136"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="172">
         <v>6</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="172">
         <v>7</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="172">
         <v>10</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="172">
         <v>11</v>
       </c>
-      <c r="M10" s="33">
+      <c r="M10" s="172">
         <v>12</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="172">
         <v>13</v>
       </c>
-      <c r="O10" s="33">
+      <c r="O10" s="172">
         <v>14</v>
       </c>
-      <c r="P10" s="33">
+      <c r="P10" s="172">
         <v>17</v>
       </c>
-      <c r="Q10" s="33">
+      <c r="Q10" s="172">
         <v>18</v>
       </c>
-      <c r="R10" s="33">
+      <c r="R10" s="172">
         <v>19</v>
       </c>
-      <c r="S10" s="33">
+      <c r="S10" s="172">
         <v>20</v>
       </c>
-      <c r="T10" s="33">
+      <c r="T10" s="172">
         <v>21</v>
       </c>
-      <c r="U10" s="33">
+      <c r="U10" s="172">
         <v>24</v>
       </c>
       <c r="V10" s="33">
@@ -2928,7 +2943,7 @@
       <c r="BQ10" s="33">
         <v>31</v>
       </c>
-      <c r="BR10" s="138"/>
+      <c r="BR10" s="158"/>
       <c r="BS10" s="34"/>
       <c r="BT10" s="34"/>
       <c r="BU10" s="34"/>
@@ -2940,15 +2955,15 @@
     </row>
     <row r="11" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34"/>
-      <c r="B11" s="147">
+      <c r="B11" s="137">
         <v>1</v>
       </c>
-      <c r="C11" s="148" t="s">
+      <c r="C11" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="135"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
       <c r="G11" s="66" t="s">
         <v>15</v>
       </c>
@@ -2958,7 +2973,7 @@
       <c r="I11" s="103"/>
       <c r="J11" s="103"/>
       <c r="K11" s="103"/>
-      <c r="L11" s="160"/>
+      <c r="L11" s="126"/>
       <c r="M11" s="103"/>
       <c r="N11" s="103"/>
       <c r="O11" s="103"/>
@@ -3016,7 +3031,7 @@
       <c r="BO11" s="35"/>
       <c r="BP11" s="35"/>
       <c r="BQ11" s="35"/>
-      <c r="BR11" s="138"/>
+      <c r="BR11" s="158"/>
       <c r="BS11" s="31"/>
       <c r="BT11" s="31"/>
       <c r="BU11" s="31"/>
@@ -3028,11 +3043,11 @@
     </row>
     <row r="12" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22"/>
-      <c r="B12" s="135"/>
-      <c r="C12" s="135"/>
-      <c r="D12" s="135"/>
-      <c r="E12" s="135"/>
-      <c r="F12" s="135"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="136"/>
       <c r="G12" s="66" t="s">
         <v>32</v>
       </c>
@@ -3042,7 +3057,7 @@
       <c r="I12" s="103"/>
       <c r="J12" s="103"/>
       <c r="K12" s="103"/>
-      <c r="L12" s="160"/>
+      <c r="L12" s="126"/>
       <c r="M12" s="103"/>
       <c r="N12" s="103"/>
       <c r="O12" s="103"/>
@@ -3100,7 +3115,7 @@
       <c r="BO12" s="35"/>
       <c r="BP12" s="35"/>
       <c r="BQ12" s="35"/>
-      <c r="BR12" s="138"/>
+      <c r="BR12" s="158"/>
       <c r="BS12" s="36"/>
       <c r="BT12" s="36"/>
       <c r="BU12" s="36"/>
@@ -3112,11 +3127,11 @@
     </row>
     <row r="13" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22"/>
-      <c r="B13" s="135"/>
-      <c r="C13" s="135"/>
-      <c r="D13" s="135"/>
-      <c r="E13" s="135"/>
-      <c r="F13" s="135"/>
+      <c r="B13" s="136"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="136"/>
+      <c r="E13" s="136"/>
+      <c r="F13" s="136"/>
       <c r="G13" s="66" t="s">
         <v>74</v>
       </c>
@@ -3126,7 +3141,7 @@
       <c r="I13" s="103"/>
       <c r="J13" s="103"/>
       <c r="K13" s="103"/>
-      <c r="L13" s="168"/>
+      <c r="L13" s="133"/>
       <c r="M13" s="103"/>
       <c r="N13" s="103"/>
       <c r="O13" s="103"/>
@@ -3184,7 +3199,7 @@
       <c r="BO13" s="35"/>
       <c r="BP13" s="35"/>
       <c r="BQ13" s="35"/>
-      <c r="BR13" s="138"/>
+      <c r="BR13" s="158"/>
       <c r="BS13" s="36"/>
       <c r="BT13" s="36"/>
       <c r="BU13" s="36"/>
@@ -3196,11 +3211,11 @@
     </row>
     <row r="14" spans="1:78" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="135"/>
-      <c r="C14" s="149"/>
-      <c r="D14" s="149"/>
-      <c r="E14" s="149"/>
-      <c r="F14" s="149"/>
+      <c r="B14" s="136"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="139"/>
+      <c r="E14" s="139"/>
+      <c r="F14" s="139"/>
       <c r="G14" s="68" t="s">
         <v>101</v>
       </c>
@@ -3210,7 +3225,7 @@
       <c r="I14" s="105"/>
       <c r="J14" s="105"/>
       <c r="K14" s="105"/>
-      <c r="L14" s="161"/>
+      <c r="L14" s="127"/>
       <c r="M14" s="105"/>
       <c r="N14" s="105"/>
       <c r="O14" s="105"/>
@@ -3268,7 +3283,7 @@
       <c r="BO14" s="37"/>
       <c r="BP14" s="37"/>
       <c r="BQ14" s="37"/>
-      <c r="BR14" s="138"/>
+      <c r="BR14" s="158"/>
       <c r="BS14" s="36"/>
       <c r="BT14" s="36"/>
       <c r="BU14" s="36"/>
@@ -3280,15 +3295,15 @@
     </row>
     <row r="15" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
-      <c r="B15" s="150">
+      <c r="B15" s="140">
         <v>2</v>
       </c>
-      <c r="C15" s="151" t="s">
+      <c r="C15" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
-      <c r="F15" s="135"/>
+      <c r="D15" s="136"/>
+      <c r="E15" s="136"/>
+      <c r="F15" s="136"/>
       <c r="G15" s="69" t="s">
         <v>33</v>
       </c>
@@ -3298,7 +3313,7 @@
       <c r="I15" s="38"/>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
-      <c r="L15" s="169"/>
+      <c r="L15" s="134"/>
       <c r="M15" s="123"/>
       <c r="N15" s="123"/>
       <c r="O15" s="123"/>
@@ -3356,7 +3371,7 @@
       <c r="BO15" s="38"/>
       <c r="BP15" s="38"/>
       <c r="BQ15" s="38"/>
-      <c r="BR15" s="138"/>
+      <c r="BR15" s="158"/>
       <c r="BS15" s="39"/>
       <c r="BT15" s="22"/>
       <c r="BU15" s="22"/>
@@ -3368,11 +3383,11 @@
     </row>
     <row r="16" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22"/>
-      <c r="B16" s="135"/>
-      <c r="C16" s="135"/>
-      <c r="D16" s="135"/>
-      <c r="E16" s="135"/>
-      <c r="F16" s="135"/>
+      <c r="B16" s="136"/>
+      <c r="C16" s="136"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="136"/>
+      <c r="F16" s="136"/>
       <c r="G16" s="69" t="s">
         <v>54</v>
       </c>
@@ -3382,7 +3397,7 @@
       <c r="I16" s="40"/>
       <c r="J16" s="40"/>
       <c r="K16" s="40"/>
-      <c r="L16" s="162"/>
+      <c r="L16" s="128"/>
       <c r="M16" s="40"/>
       <c r="N16" s="40"/>
       <c r="O16" s="40"/>
@@ -3440,7 +3455,7 @@
       <c r="BO16" s="40"/>
       <c r="BP16" s="40"/>
       <c r="BQ16" s="40"/>
-      <c r="BR16" s="138"/>
+      <c r="BR16" s="158"/>
       <c r="BS16" s="39"/>
       <c r="BT16" s="22"/>
       <c r="BU16" s="22"/>
@@ -3452,11 +3467,11 @@
     </row>
     <row r="17" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22"/>
-      <c r="B17" s="135"/>
-      <c r="C17" s="135"/>
-      <c r="D17" s="135"/>
-      <c r="E17" s="135"/>
-      <c r="F17" s="135"/>
+      <c r="B17" s="136"/>
+      <c r="C17" s="136"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
       <c r="G17" s="69" t="s">
         <v>34</v>
       </c>
@@ -3466,7 +3481,7 @@
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="162"/>
+      <c r="L17" s="128"/>
       <c r="M17" s="40"/>
       <c r="N17" s="40"/>
       <c r="O17" s="40"/>
@@ -3524,7 +3539,7 @@
       <c r="BO17" s="40"/>
       <c r="BP17" s="40"/>
       <c r="BQ17" s="40"/>
-      <c r="BR17" s="138"/>
+      <c r="BR17" s="158"/>
       <c r="BS17" s="39"/>
       <c r="BT17" s="22"/>
       <c r="BU17" s="22"/>
@@ -3536,11 +3551,11 @@
     </row>
     <row r="18" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22"/>
-      <c r="B18" s="135"/>
-      <c r="C18" s="135"/>
-      <c r="D18" s="135"/>
-      <c r="E18" s="135"/>
-      <c r="F18" s="135"/>
+      <c r="B18" s="136"/>
+      <c r="C18" s="136"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="136"/>
       <c r="G18" s="69" t="s">
         <v>89</v>
       </c>
@@ -3550,7 +3565,7 @@
       <c r="I18" s="40"/>
       <c r="J18" s="40"/>
       <c r="K18" s="40"/>
-      <c r="L18" s="163" t="s">
+      <c r="L18" s="129" t="s">
         <v>102</v>
       </c>
       <c r="M18" s="85"/>
@@ -3610,7 +3625,7 @@
       <c r="BO18" s="40"/>
       <c r="BP18" s="40"/>
       <c r="BQ18" s="40"/>
-      <c r="BR18" s="138"/>
+      <c r="BR18" s="158"/>
       <c r="BS18" s="39"/>
       <c r="BT18" s="22"/>
       <c r="BU18" s="22"/>
@@ -3622,11 +3637,11 @@
     </row>
     <row r="19" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22"/>
-      <c r="B19" s="135"/>
-      <c r="C19" s="135"/>
-      <c r="D19" s="135"/>
-      <c r="E19" s="135"/>
-      <c r="F19" s="135"/>
+      <c r="B19" s="136"/>
+      <c r="C19" s="136"/>
+      <c r="D19" s="136"/>
+      <c r="E19" s="136"/>
+      <c r="F19" s="136"/>
       <c r="G19" s="69" t="s">
         <v>35</v>
       </c>
@@ -3636,7 +3651,7 @@
       <c r="I19" s="40"/>
       <c r="J19" s="40"/>
       <c r="K19" s="40"/>
-      <c r="L19" s="163" t="s">
+      <c r="L19" s="129" t="s">
         <v>102</v>
       </c>
       <c r="M19" s="85"/>
@@ -3696,7 +3711,7 @@
       <c r="BO19" s="40"/>
       <c r="BP19" s="40"/>
       <c r="BQ19" s="40"/>
-      <c r="BR19" s="138"/>
+      <c r="BR19" s="158"/>
       <c r="BS19" s="39"/>
       <c r="BT19" s="22"/>
       <c r="BU19" s="22"/>
@@ -3708,11 +3723,11 @@
     </row>
     <row r="20" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22"/>
-      <c r="B20" s="135"/>
-      <c r="C20" s="135"/>
-      <c r="D20" s="135"/>
-      <c r="E20" s="135"/>
-      <c r="F20" s="135"/>
+      <c r="B20" s="136"/>
+      <c r="C20" s="136"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
       <c r="G20" s="69" t="s">
         <v>99</v>
       </c>
@@ -3722,7 +3737,7 @@
       <c r="I20" s="40"/>
       <c r="J20" s="40"/>
       <c r="K20" s="40"/>
-      <c r="L20" s="164"/>
+      <c r="L20" s="128"/>
       <c r="M20" s="85"/>
       <c r="N20" s="85"/>
       <c r="O20" s="85"/>
@@ -3780,7 +3795,7 @@
       <c r="BO20" s="40"/>
       <c r="BP20" s="40"/>
       <c r="BQ20" s="40"/>
-      <c r="BR20" s="138"/>
+      <c r="BR20" s="158"/>
       <c r="BS20" s="39"/>
       <c r="BT20" s="22"/>
       <c r="BU20" s="22"/>
@@ -3792,11 +3807,11 @@
     </row>
     <row r="21" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22"/>
-      <c r="B21" s="135"/>
-      <c r="C21" s="135"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="135"/>
-      <c r="F21" s="135"/>
+      <c r="B21" s="136"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="136"/>
       <c r="G21" s="69" t="s">
         <v>36</v>
       </c>
@@ -3806,7 +3821,7 @@
       <c r="I21" s="40"/>
       <c r="J21" s="40"/>
       <c r="K21" s="40"/>
-      <c r="L21" s="162"/>
+      <c r="L21" s="128"/>
       <c r="M21" s="85"/>
       <c r="N21" s="85"/>
       <c r="O21" s="85"/>
@@ -3864,7 +3879,7 @@
       <c r="BO21" s="40"/>
       <c r="BP21" s="40"/>
       <c r="BQ21" s="40"/>
-      <c r="BR21" s="138"/>
+      <c r="BR21" s="158"/>
       <c r="BS21" s="39"/>
       <c r="BT21" s="22"/>
       <c r="BU21" s="22"/>
@@ -3876,11 +3891,11 @@
     </row>
     <row r="22" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="22"/>
-      <c r="B22" s="135"/>
-      <c r="C22" s="135"/>
-      <c r="D22" s="135"/>
-      <c r="E22" s="135"/>
-      <c r="F22" s="135"/>
+      <c r="B22" s="136"/>
+      <c r="C22" s="136"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="136"/>
       <c r="G22" s="108" t="s">
         <v>38</v>
       </c>
@@ -3948,7 +3963,7 @@
       <c r="BO22" s="40"/>
       <c r="BP22" s="40"/>
       <c r="BQ22" s="40"/>
-      <c r="BR22" s="138"/>
+      <c r="BR22" s="158"/>
       <c r="BS22" s="39"/>
       <c r="BT22" s="22"/>
       <c r="BU22" s="22"/>
@@ -3960,11 +3975,11 @@
     </row>
     <row r="23" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="22"/>
-      <c r="B23" s="135"/>
-      <c r="C23" s="135"/>
-      <c r="D23" s="135"/>
-      <c r="E23" s="135"/>
-      <c r="F23" s="135"/>
+      <c r="B23" s="136"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="136"/>
+      <c r="F23" s="136"/>
       <c r="G23" s="109" t="s">
         <v>90</v>
       </c>
@@ -4032,7 +4047,7 @@
       <c r="BO23" s="107"/>
       <c r="BP23" s="107"/>
       <c r="BQ23" s="107"/>
-      <c r="BR23" s="138"/>
+      <c r="BR23" s="158"/>
       <c r="BS23" s="39"/>
       <c r="BT23" s="22"/>
       <c r="BU23" s="22"/>
@@ -4044,11 +4059,11 @@
     </row>
     <row r="24" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="22"/>
-      <c r="B24" s="135"/>
-      <c r="C24" s="135"/>
-      <c r="D24" s="135"/>
-      <c r="E24" s="135"/>
-      <c r="F24" s="135"/>
+      <c r="B24" s="136"/>
+      <c r="C24" s="136"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="136"/>
+      <c r="F24" s="136"/>
       <c r="G24" s="109" t="s">
         <v>39</v>
       </c>
@@ -4116,7 +4131,7 @@
       <c r="BO24" s="107"/>
       <c r="BP24" s="107"/>
       <c r="BQ24" s="107"/>
-      <c r="BR24" s="138"/>
+      <c r="BR24" s="158"/>
       <c r="BS24" s="39"/>
       <c r="BT24" s="22"/>
       <c r="BU24" s="22"/>
@@ -4128,11 +4143,11 @@
     </row>
     <row r="25" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22"/>
-      <c r="B25" s="135"/>
-      <c r="C25" s="135"/>
-      <c r="D25" s="135"/>
-      <c r="E25" s="135"/>
-      <c r="F25" s="135"/>
+      <c r="B25" s="136"/>
+      <c r="C25" s="136"/>
+      <c r="D25" s="136"/>
+      <c r="E25" s="136"/>
+      <c r="F25" s="136"/>
       <c r="G25" s="109" t="s">
         <v>40</v>
       </c>
@@ -4200,7 +4215,7 @@
       <c r="BO25" s="107"/>
       <c r="BP25" s="107"/>
       <c r="BQ25" s="107"/>
-      <c r="BR25" s="138"/>
+      <c r="BR25" s="158"/>
       <c r="BS25" s="39"/>
       <c r="BT25" s="22"/>
       <c r="BU25" s="22"/>
@@ -4212,11 +4227,11 @@
     </row>
     <row r="26" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="22"/>
-      <c r="B26" s="135"/>
-      <c r="C26" s="135"/>
-      <c r="D26" s="135"/>
-      <c r="E26" s="135"/>
-      <c r="F26" s="135"/>
+      <c r="B26" s="136"/>
+      <c r="C26" s="136"/>
+      <c r="D26" s="136"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
       <c r="G26" s="109" t="s">
         <v>41</v>
       </c>
@@ -4284,7 +4299,7 @@
       <c r="BO26" s="107"/>
       <c r="BP26" s="107"/>
       <c r="BQ26" s="107"/>
-      <c r="BR26" s="138"/>
+      <c r="BR26" s="158"/>
       <c r="BS26" s="39"/>
       <c r="BT26" s="22"/>
       <c r="BU26" s="22"/>
@@ -4296,11 +4311,11 @@
     </row>
     <row r="27" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
-      <c r="B27" s="135"/>
-      <c r="C27" s="135"/>
-      <c r="D27" s="135"/>
-      <c r="E27" s="135"/>
-      <c r="F27" s="135"/>
+      <c r="B27" s="136"/>
+      <c r="C27" s="136"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="136"/>
       <c r="G27" s="109" t="s">
         <v>42</v>
       </c>
@@ -4368,7 +4383,7 @@
       <c r="BO27" s="107"/>
       <c r="BP27" s="107"/>
       <c r="BQ27" s="107"/>
-      <c r="BR27" s="138"/>
+      <c r="BR27" s="158"/>
       <c r="BS27" s="39"/>
       <c r="BT27" s="22"/>
       <c r="BU27" s="22"/>
@@ -4380,11 +4395,11 @@
     </row>
     <row r="28" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="22"/>
-      <c r="B28" s="135"/>
-      <c r="C28" s="135"/>
-      <c r="D28" s="135"/>
-      <c r="E28" s="135"/>
-      <c r="F28" s="135"/>
+      <c r="B28" s="136"/>
+      <c r="C28" s="136"/>
+      <c r="D28" s="136"/>
+      <c r="E28" s="136"/>
+      <c r="F28" s="136"/>
       <c r="G28" s="109" t="s">
         <v>37</v>
       </c>
@@ -4452,7 +4467,7 @@
       <c r="BO28" s="107"/>
       <c r="BP28" s="107"/>
       <c r="BQ28" s="107"/>
-      <c r="BR28" s="138"/>
+      <c r="BR28" s="158"/>
       <c r="BS28" s="39"/>
       <c r="BT28" s="22"/>
       <c r="BU28" s="22"/>
@@ -4464,11 +4479,11 @@
     </row>
     <row r="29" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22"/>
-      <c r="B29" s="135"/>
-      <c r="C29" s="135"/>
-      <c r="D29" s="135"/>
-      <c r="E29" s="135"/>
-      <c r="F29" s="135"/>
+      <c r="B29" s="136"/>
+      <c r="C29" s="136"/>
+      <c r="D29" s="136"/>
+      <c r="E29" s="136"/>
+      <c r="F29" s="136"/>
       <c r="G29" s="109" t="s">
         <v>43</v>
       </c>
@@ -4536,7 +4551,7 @@
       <c r="BO29" s="107"/>
       <c r="BP29" s="107"/>
       <c r="BQ29" s="107"/>
-      <c r="BR29" s="138"/>
+      <c r="BR29" s="158"/>
       <c r="BS29" s="39"/>
       <c r="BT29" s="22"/>
       <c r="BU29" s="22"/>
@@ -4548,11 +4563,11 @@
     </row>
     <row r="30" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22"/>
-      <c r="B30" s="135"/>
-      <c r="C30" s="135"/>
-      <c r="D30" s="135"/>
-      <c r="E30" s="135"/>
-      <c r="F30" s="135"/>
+      <c r="B30" s="136"/>
+      <c r="C30" s="136"/>
+      <c r="D30" s="136"/>
+      <c r="E30" s="136"/>
+      <c r="F30" s="136"/>
       <c r="G30" s="109" t="s">
         <v>44</v>
       </c>
@@ -4620,7 +4635,7 @@
       <c r="BO30" s="107"/>
       <c r="BP30" s="107"/>
       <c r="BQ30" s="107"/>
-      <c r="BR30" s="138"/>
+      <c r="BR30" s="158"/>
       <c r="BS30" s="39"/>
       <c r="BT30" s="22"/>
       <c r="BU30" s="22"/>
@@ -4632,11 +4647,11 @@
     </row>
     <row r="31" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22"/>
-      <c r="B31" s="135"/>
-      <c r="C31" s="135"/>
-      <c r="D31" s="135"/>
-      <c r="E31" s="135"/>
-      <c r="F31" s="135"/>
+      <c r="B31" s="136"/>
+      <c r="C31" s="136"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="136"/>
       <c r="G31" s="109" t="s">
         <v>45</v>
       </c>
@@ -4704,7 +4719,7 @@
       <c r="BO31" s="107"/>
       <c r="BP31" s="107"/>
       <c r="BQ31" s="107"/>
-      <c r="BR31" s="138"/>
+      <c r="BR31" s="158"/>
       <c r="BS31" s="39"/>
       <c r="BT31" s="22"/>
       <c r="BU31" s="22"/>
@@ -4716,11 +4731,11 @@
     </row>
     <row r="32" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="22"/>
-      <c r="B32" s="135"/>
-      <c r="C32" s="135"/>
-      <c r="D32" s="135"/>
-      <c r="E32" s="135"/>
-      <c r="F32" s="135"/>
+      <c r="B32" s="136"/>
+      <c r="C32" s="136"/>
+      <c r="D32" s="136"/>
+      <c r="E32" s="136"/>
+      <c r="F32" s="136"/>
       <c r="G32" s="110" t="s">
         <v>46</v>
       </c>
@@ -4788,7 +4803,7 @@
       <c r="BO32" s="107"/>
       <c r="BP32" s="107"/>
       <c r="BQ32" s="107"/>
-      <c r="BR32" s="138"/>
+      <c r="BR32" s="158"/>
       <c r="BS32" s="39"/>
       <c r="BT32" s="22"/>
       <c r="BU32" s="22"/>
@@ -4800,11 +4815,11 @@
     </row>
     <row r="33" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22"/>
-      <c r="B33" s="135"/>
-      <c r="C33" s="135"/>
-      <c r="D33" s="135"/>
-      <c r="E33" s="135"/>
-      <c r="F33" s="135"/>
+      <c r="B33" s="136"/>
+      <c r="C33" s="136"/>
+      <c r="D33" s="136"/>
+      <c r="E33" s="136"/>
+      <c r="F33" s="136"/>
       <c r="G33" s="109" t="s">
         <v>47</v>
       </c>
@@ -4830,7 +4845,7 @@
       <c r="Y33" s="107"/>
       <c r="Z33" s="107"/>
       <c r="AA33" s="107"/>
-      <c r="AB33" s="111"/>
+      <c r="AB33" s="169"/>
       <c r="AC33" s="107"/>
       <c r="AD33" s="107"/>
       <c r="AE33" s="107"/>
@@ -4872,7 +4887,7 @@
       <c r="BO33" s="107"/>
       <c r="BP33" s="107"/>
       <c r="BQ33" s="107"/>
-      <c r="BR33" s="138"/>
+      <c r="BR33" s="158"/>
       <c r="BS33" s="39"/>
       <c r="BT33" s="22"/>
       <c r="BU33" s="22"/>
@@ -4884,11 +4899,11 @@
     </row>
     <row r="34" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22"/>
-      <c r="B34" s="135"/>
-      <c r="C34" s="135"/>
-      <c r="D34" s="135"/>
-      <c r="E34" s="135"/>
-      <c r="F34" s="135"/>
+      <c r="B34" s="136"/>
+      <c r="C34" s="136"/>
+      <c r="D34" s="136"/>
+      <c r="E34" s="136"/>
+      <c r="F34" s="136"/>
       <c r="G34" s="109" t="s">
         <v>48</v>
       </c>
@@ -4915,7 +4930,7 @@
       <c r="Z34" s="107"/>
       <c r="AA34" s="107"/>
       <c r="AB34" s="107"/>
-      <c r="AC34" s="111"/>
+      <c r="AC34" s="169"/>
       <c r="AD34" s="107"/>
       <c r="AE34" s="107"/>
       <c r="AF34" s="107"/>
@@ -4956,7 +4971,7 @@
       <c r="BO34" s="107"/>
       <c r="BP34" s="107"/>
       <c r="BQ34" s="107"/>
-      <c r="BR34" s="138"/>
+      <c r="BR34" s="158"/>
       <c r="BS34" s="39"/>
       <c r="BT34" s="22"/>
       <c r="BU34" s="22"/>
@@ -4968,11 +4983,11 @@
     </row>
     <row r="35" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22"/>
-      <c r="B35" s="135"/>
-      <c r="C35" s="135"/>
-      <c r="D35" s="135"/>
-      <c r="E35" s="135"/>
-      <c r="F35" s="135"/>
+      <c r="B35" s="136"/>
+      <c r="C35" s="136"/>
+      <c r="D35" s="136"/>
+      <c r="E35" s="136"/>
+      <c r="F35" s="136"/>
       <c r="G35" s="109" t="s">
         <v>49</v>
       </c>
@@ -5000,7 +5015,7 @@
       <c r="AA35" s="107"/>
       <c r="AB35" s="107"/>
       <c r="AC35" s="107"/>
-      <c r="AD35" s="111"/>
+      <c r="AD35" s="169"/>
       <c r="AE35" s="107"/>
       <c r="AF35" s="107"/>
       <c r="AG35" s="107"/>
@@ -5040,7 +5055,7 @@
       <c r="BO35" s="107"/>
       <c r="BP35" s="107"/>
       <c r="BQ35" s="107"/>
-      <c r="BR35" s="138"/>
+      <c r="BR35" s="158"/>
       <c r="BS35" s="39"/>
       <c r="BT35" s="22"/>
       <c r="BU35" s="22"/>
@@ -5052,11 +5067,11 @@
     </row>
     <row r="36" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22"/>
-      <c r="B36" s="135"/>
-      <c r="C36" s="135"/>
-      <c r="D36" s="135"/>
-      <c r="E36" s="135"/>
-      <c r="F36" s="135"/>
+      <c r="B36" s="136"/>
+      <c r="C36" s="136"/>
+      <c r="D36" s="136"/>
+      <c r="E36" s="136"/>
+      <c r="F36" s="136"/>
       <c r="G36" s="109" t="s">
         <v>51</v>
       </c>
@@ -5085,7 +5100,7 @@
       <c r="AB36" s="107"/>
       <c r="AC36" s="107"/>
       <c r="AD36" s="107"/>
-      <c r="AE36" s="111"/>
+      <c r="AE36" s="169"/>
       <c r="AF36" s="107"/>
       <c r="AG36" s="107"/>
       <c r="AH36" s="107"/>
@@ -5124,7 +5139,7 @@
       <c r="BO36" s="107"/>
       <c r="BP36" s="107"/>
       <c r="BQ36" s="107"/>
-      <c r="BR36" s="138"/>
+      <c r="BR36" s="158"/>
       <c r="BS36" s="39"/>
       <c r="BT36" s="22"/>
       <c r="BU36" s="22"/>
@@ -5136,11 +5151,11 @@
     </row>
     <row r="37" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22"/>
-      <c r="B37" s="135"/>
-      <c r="C37" s="135"/>
-      <c r="D37" s="135"/>
-      <c r="E37" s="135"/>
-      <c r="F37" s="135"/>
+      <c r="B37" s="136"/>
+      <c r="C37" s="136"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="136"/>
+      <c r="F37" s="136"/>
       <c r="G37" s="109" t="s">
         <v>50</v>
       </c>
@@ -5170,7 +5185,7 @@
       <c r="AC37" s="107"/>
       <c r="AD37" s="107"/>
       <c r="AE37" s="107"/>
-      <c r="AF37" s="111"/>
+      <c r="AF37" s="169"/>
       <c r="AG37" s="107"/>
       <c r="AH37" s="107"/>
       <c r="AI37" s="107"/>
@@ -5208,7 +5223,7 @@
       <c r="BO37" s="107"/>
       <c r="BP37" s="107"/>
       <c r="BQ37" s="107"/>
-      <c r="BR37" s="138"/>
+      <c r="BR37" s="158"/>
       <c r="BS37" s="39"/>
       <c r="BT37" s="22"/>
       <c r="BU37" s="22"/>
@@ -5220,11 +5235,11 @@
     </row>
     <row r="38" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="22"/>
-      <c r="B38" s="135"/>
-      <c r="C38" s="135"/>
-      <c r="D38" s="135"/>
-      <c r="E38" s="135"/>
-      <c r="F38" s="135"/>
+      <c r="B38" s="136"/>
+      <c r="C38" s="136"/>
+      <c r="D38" s="136"/>
+      <c r="E38" s="136"/>
+      <c r="F38" s="136"/>
       <c r="G38" s="109" t="s">
         <v>52</v>
       </c>
@@ -5292,7 +5307,7 @@
       <c r="BO38" s="107"/>
       <c r="BP38" s="107"/>
       <c r="BQ38" s="107"/>
-      <c r="BR38" s="138"/>
+      <c r="BR38" s="158"/>
       <c r="BS38" s="39"/>
       <c r="BT38" s="22"/>
       <c r="BU38" s="22"/>
@@ -5304,11 +5319,11 @@
     </row>
     <row r="39" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22"/>
-      <c r="B39" s="135"/>
-      <c r="C39" s="135"/>
-      <c r="D39" s="135"/>
-      <c r="E39" s="135"/>
-      <c r="F39" s="135"/>
+      <c r="B39" s="136"/>
+      <c r="C39" s="136"/>
+      <c r="D39" s="136"/>
+      <c r="E39" s="136"/>
+      <c r="F39" s="136"/>
       <c r="G39" s="110" t="s">
         <v>53</v>
       </c>
@@ -5376,7 +5391,7 @@
       <c r="BO39" s="107"/>
       <c r="BP39" s="107"/>
       <c r="BQ39" s="107"/>
-      <c r="BR39" s="138"/>
+      <c r="BR39" s="158"/>
       <c r="BS39" s="39"/>
       <c r="BT39" s="22"/>
       <c r="BU39" s="22"/>
@@ -5388,11 +5403,11 @@
     </row>
     <row r="40" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="22"/>
-      <c r="B40" s="135"/>
-      <c r="C40" s="135"/>
-      <c r="D40" s="135"/>
-      <c r="E40" s="135"/>
-      <c r="F40" s="135"/>
+      <c r="B40" s="136"/>
+      <c r="C40" s="136"/>
+      <c r="D40" s="136"/>
+      <c r="E40" s="136"/>
+      <c r="F40" s="136"/>
       <c r="G40" s="69" t="s">
         <v>55</v>
       </c>
@@ -5460,7 +5475,7 @@
       <c r="BO40" s="107"/>
       <c r="BP40" s="107"/>
       <c r="BQ40" s="107"/>
-      <c r="BR40" s="138"/>
+      <c r="BR40" s="158"/>
       <c r="BS40" s="39"/>
       <c r="BT40" s="22"/>
       <c r="BU40" s="22"/>
@@ -5472,11 +5487,11 @@
     </row>
     <row r="41" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="22"/>
-      <c r="B41" s="135"/>
-      <c r="C41" s="135"/>
-      <c r="D41" s="135"/>
-      <c r="E41" s="135"/>
-      <c r="F41" s="135"/>
+      <c r="B41" s="136"/>
+      <c r="C41" s="136"/>
+      <c r="D41" s="136"/>
+      <c r="E41" s="136"/>
+      <c r="F41" s="136"/>
       <c r="G41" s="69" t="s">
         <v>56</v>
       </c>
@@ -5544,7 +5559,7 @@
       <c r="BO41" s="107"/>
       <c r="BP41" s="107"/>
       <c r="BQ41" s="107"/>
-      <c r="BR41" s="138"/>
+      <c r="BR41" s="158"/>
       <c r="BS41" s="39"/>
       <c r="BT41" s="22"/>
       <c r="BU41" s="22"/>
@@ -5556,11 +5571,11 @@
     </row>
     <row r="42" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="22"/>
-      <c r="B42" s="135"/>
-      <c r="C42" s="135"/>
-      <c r="D42" s="135"/>
-      <c r="E42" s="135"/>
-      <c r="F42" s="135"/>
+      <c r="B42" s="136"/>
+      <c r="C42" s="136"/>
+      <c r="D42" s="136"/>
+      <c r="E42" s="136"/>
+      <c r="F42" s="136"/>
       <c r="G42" s="69" t="s">
         <v>57</v>
       </c>
@@ -5628,7 +5643,7 @@
       <c r="BO42" s="107"/>
       <c r="BP42" s="107"/>
       <c r="BQ42" s="107"/>
-      <c r="BR42" s="138"/>
+      <c r="BR42" s="158"/>
       <c r="BS42" s="39"/>
       <c r="BT42" s="22"/>
       <c r="BU42" s="22"/>
@@ -5640,11 +5655,11 @@
     </row>
     <row r="43" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="22"/>
-      <c r="B43" s="135"/>
-      <c r="C43" s="135"/>
-      <c r="D43" s="135"/>
-      <c r="E43" s="135"/>
-      <c r="F43" s="135"/>
+      <c r="B43" s="136"/>
+      <c r="C43" s="136"/>
+      <c r="D43" s="136"/>
+      <c r="E43" s="136"/>
+      <c r="F43" s="136"/>
       <c r="G43" s="69" t="s">
         <v>91</v>
       </c>
@@ -5712,7 +5727,7 @@
       <c r="BO43" s="107"/>
       <c r="BP43" s="107"/>
       <c r="BQ43" s="107"/>
-      <c r="BR43" s="138"/>
+      <c r="BR43" s="158"/>
       <c r="BS43" s="39"/>
       <c r="BT43" s="22"/>
       <c r="BU43" s="22"/>
@@ -5724,11 +5739,11 @@
     </row>
     <row r="44" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="22"/>
-      <c r="B44" s="135"/>
-      <c r="C44" s="135"/>
-      <c r="D44" s="135"/>
-      <c r="E44" s="135"/>
-      <c r="F44" s="135"/>
+      <c r="B44" s="136"/>
+      <c r="C44" s="136"/>
+      <c r="D44" s="136"/>
+      <c r="E44" s="136"/>
+      <c r="F44" s="136"/>
       <c r="G44" s="69" t="s">
         <v>92</v>
       </c>
@@ -5796,7 +5811,7 @@
       <c r="BO44" s="107"/>
       <c r="BP44" s="107"/>
       <c r="BQ44" s="107"/>
-      <c r="BR44" s="138"/>
+      <c r="BR44" s="158"/>
       <c r="BS44" s="39"/>
       <c r="BT44" s="22"/>
       <c r="BU44" s="22"/>
@@ -5808,11 +5823,11 @@
     </row>
     <row r="45" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="22"/>
-      <c r="B45" s="135"/>
-      <c r="C45" s="135"/>
-      <c r="D45" s="135"/>
-      <c r="E45" s="135"/>
-      <c r="F45" s="135"/>
+      <c r="B45" s="136"/>
+      <c r="C45" s="136"/>
+      <c r="D45" s="136"/>
+      <c r="E45" s="136"/>
+      <c r="F45" s="136"/>
       <c r="G45" s="69" t="s">
         <v>58</v>
       </c>
@@ -5880,7 +5895,7 @@
       <c r="BO45" s="107"/>
       <c r="BP45" s="107"/>
       <c r="BQ45" s="107"/>
-      <c r="BR45" s="138"/>
+      <c r="BR45" s="158"/>
       <c r="BS45" s="39"/>
       <c r="BT45" s="22"/>
       <c r="BU45" s="22"/>
@@ -5892,11 +5907,11 @@
     </row>
     <row r="46" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="22"/>
-      <c r="B46" s="135"/>
-      <c r="C46" s="135"/>
-      <c r="D46" s="135"/>
-      <c r="E46" s="135"/>
-      <c r="F46" s="135"/>
+      <c r="B46" s="136"/>
+      <c r="C46" s="136"/>
+      <c r="D46" s="136"/>
+      <c r="E46" s="136"/>
+      <c r="F46" s="136"/>
       <c r="G46" s="69" t="s">
         <v>59</v>
       </c>
@@ -5964,7 +5979,7 @@
       <c r="BO46" s="107"/>
       <c r="BP46" s="107"/>
       <c r="BQ46" s="107"/>
-      <c r="BR46" s="138"/>
+      <c r="BR46" s="158"/>
       <c r="BS46" s="39"/>
       <c r="BT46" s="22"/>
       <c r="BU46" s="22"/>
@@ -5976,11 +5991,11 @@
     </row>
     <row r="47" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="22"/>
-      <c r="B47" s="135"/>
-      <c r="C47" s="135"/>
-      <c r="D47" s="135"/>
-      <c r="E47" s="135"/>
-      <c r="F47" s="135"/>
+      <c r="B47" s="136"/>
+      <c r="C47" s="136"/>
+      <c r="D47" s="136"/>
+      <c r="E47" s="136"/>
+      <c r="F47" s="136"/>
       <c r="G47" s="69" t="s">
         <v>60</v>
       </c>
@@ -6048,7 +6063,7 @@
       <c r="BO47" s="107"/>
       <c r="BP47" s="107"/>
       <c r="BQ47" s="107"/>
-      <c r="BR47" s="138"/>
+      <c r="BR47" s="158"/>
       <c r="BS47" s="39"/>
       <c r="BT47" s="22"/>
       <c r="BU47" s="22"/>
@@ -6060,11 +6075,11 @@
     </row>
     <row r="48" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="22"/>
-      <c r="B48" s="135"/>
-      <c r="C48" s="135"/>
-      <c r="D48" s="135"/>
-      <c r="E48" s="135"/>
-      <c r="F48" s="135"/>
+      <c r="B48" s="136"/>
+      <c r="C48" s="136"/>
+      <c r="D48" s="136"/>
+      <c r="E48" s="136"/>
+      <c r="F48" s="136"/>
       <c r="G48" s="69" t="s">
         <v>61</v>
       </c>
@@ -6103,7 +6118,7 @@
       <c r="AL48" s="107"/>
       <c r="AM48" s="107"/>
       <c r="AN48" s="107"/>
-      <c r="AO48" s="112"/>
+      <c r="AO48" s="169"/>
       <c r="AP48" s="107"/>
       <c r="AQ48" s="107"/>
       <c r="AR48" s="107"/>
@@ -6132,7 +6147,7 @@
       <c r="BO48" s="107"/>
       <c r="BP48" s="107"/>
       <c r="BQ48" s="107"/>
-      <c r="BR48" s="138"/>
+      <c r="BR48" s="158"/>
       <c r="BS48" s="39"/>
       <c r="BT48" s="22"/>
       <c r="BU48" s="22"/>
@@ -6144,11 +6159,11 @@
     </row>
     <row r="49" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="22"/>
-      <c r="B49" s="135"/>
-      <c r="C49" s="135"/>
-      <c r="D49" s="135"/>
-      <c r="E49" s="135"/>
-      <c r="F49" s="135"/>
+      <c r="B49" s="136"/>
+      <c r="C49" s="136"/>
+      <c r="D49" s="136"/>
+      <c r="E49" s="136"/>
+      <c r="F49" s="136"/>
       <c r="G49" s="69" t="s">
         <v>62</v>
       </c>
@@ -6216,7 +6231,7 @@
       <c r="BO49" s="107"/>
       <c r="BP49" s="107"/>
       <c r="BQ49" s="107"/>
-      <c r="BR49" s="138"/>
+      <c r="BR49" s="158"/>
       <c r="BS49" s="39"/>
       <c r="BT49" s="22"/>
       <c r="BU49" s="22"/>
@@ -6228,11 +6243,11 @@
     </row>
     <row r="50" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="22"/>
-      <c r="B50" s="135"/>
-      <c r="C50" s="135"/>
-      <c r="D50" s="135"/>
-      <c r="E50" s="135"/>
-      <c r="F50" s="135"/>
+      <c r="B50" s="136"/>
+      <c r="C50" s="136"/>
+      <c r="D50" s="136"/>
+      <c r="E50" s="136"/>
+      <c r="F50" s="136"/>
       <c r="G50" s="69" t="s">
         <v>63</v>
       </c>
@@ -6300,7 +6315,7 @@
       <c r="BO50" s="107"/>
       <c r="BP50" s="107"/>
       <c r="BQ50" s="107"/>
-      <c r="BR50" s="138"/>
+      <c r="BR50" s="158"/>
       <c r="BS50" s="39"/>
       <c r="BT50" s="22"/>
       <c r="BU50" s="22"/>
@@ -6312,11 +6327,11 @@
     </row>
     <row r="51" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22"/>
-      <c r="B51" s="135"/>
-      <c r="C51" s="135"/>
-      <c r="D51" s="135"/>
-      <c r="E51" s="135"/>
-      <c r="F51" s="135"/>
+      <c r="B51" s="136"/>
+      <c r="C51" s="136"/>
+      <c r="D51" s="136"/>
+      <c r="E51" s="136"/>
+      <c r="F51" s="136"/>
       <c r="G51" s="69" t="s">
         <v>64</v>
       </c>
@@ -6384,7 +6399,7 @@
       <c r="BO51" s="107"/>
       <c r="BP51" s="107"/>
       <c r="BQ51" s="107"/>
-      <c r="BR51" s="138"/>
+      <c r="BR51" s="158"/>
       <c r="BS51" s="39"/>
       <c r="BT51" s="22"/>
       <c r="BU51" s="22"/>
@@ -6396,11 +6411,11 @@
     </row>
     <row r="52" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="22"/>
-      <c r="B52" s="135"/>
-      <c r="C52" s="135"/>
-      <c r="D52" s="135"/>
-      <c r="E52" s="135"/>
-      <c r="F52" s="135"/>
+      <c r="B52" s="136"/>
+      <c r="C52" s="136"/>
+      <c r="D52" s="136"/>
+      <c r="E52" s="136"/>
+      <c r="F52" s="136"/>
       <c r="G52" s="69" t="s">
         <v>93</v>
       </c>
@@ -6468,7 +6483,7 @@
       <c r="BO52" s="107"/>
       <c r="BP52" s="107"/>
       <c r="BQ52" s="107"/>
-      <c r="BR52" s="138"/>
+      <c r="BR52" s="158"/>
       <c r="BS52" s="39"/>
       <c r="BT52" s="22"/>
       <c r="BU52" s="22"/>
@@ -6480,11 +6495,11 @@
     </row>
     <row r="53" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="22"/>
-      <c r="B53" s="135"/>
-      <c r="C53" s="135"/>
-      <c r="D53" s="135"/>
-      <c r="E53" s="135"/>
-      <c r="F53" s="135"/>
+      <c r="B53" s="136"/>
+      <c r="C53" s="136"/>
+      <c r="D53" s="136"/>
+      <c r="E53" s="136"/>
+      <c r="F53" s="136"/>
       <c r="G53" s="69" t="s">
         <v>65</v>
       </c>
@@ -6552,7 +6567,7 @@
       <c r="BO53" s="107"/>
       <c r="BP53" s="107"/>
       <c r="BQ53" s="107"/>
-      <c r="BR53" s="138"/>
+      <c r="BR53" s="158"/>
       <c r="BS53" s="39"/>
       <c r="BT53" s="22"/>
       <c r="BU53" s="22"/>
@@ -6564,11 +6579,11 @@
     </row>
     <row r="54" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="22"/>
-      <c r="B54" s="135"/>
-      <c r="C54" s="135"/>
-      <c r="D54" s="135"/>
-      <c r="E54" s="135"/>
-      <c r="F54" s="135"/>
+      <c r="B54" s="136"/>
+      <c r="C54" s="136"/>
+      <c r="D54" s="136"/>
+      <c r="E54" s="136"/>
+      <c r="F54" s="136"/>
       <c r="G54" s="69" t="s">
         <v>66</v>
       </c>
@@ -6636,7 +6651,7 @@
       <c r="BO54" s="107"/>
       <c r="BP54" s="107"/>
       <c r="BQ54" s="107"/>
-      <c r="BR54" s="138"/>
+      <c r="BR54" s="158"/>
       <c r="BS54" s="39"/>
       <c r="BT54" s="22"/>
       <c r="BU54" s="22"/>
@@ -6648,11 +6663,11 @@
     </row>
     <row r="55" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="22"/>
-      <c r="B55" s="135"/>
-      <c r="C55" s="135"/>
-      <c r="D55" s="135"/>
-      <c r="E55" s="135"/>
-      <c r="F55" s="135"/>
+      <c r="B55" s="136"/>
+      <c r="C55" s="136"/>
+      <c r="D55" s="136"/>
+      <c r="E55" s="136"/>
+      <c r="F55" s="136"/>
       <c r="G55" s="69" t="s">
         <v>94</v>
       </c>
@@ -6662,16 +6677,16 @@
       <c r="I55" s="106"/>
       <c r="J55" s="106"/>
       <c r="K55" s="106"/>
-      <c r="L55" s="111"/>
-      <c r="M55" s="111"/>
-      <c r="N55" s="111"/>
-      <c r="O55" s="111"/>
-      <c r="P55" s="111"/>
-      <c r="Q55" s="111"/>
-      <c r="R55" s="111"/>
-      <c r="S55" s="111"/>
-      <c r="T55" s="111"/>
-      <c r="U55" s="111"/>
+      <c r="L55" s="171"/>
+      <c r="M55" s="171"/>
+      <c r="N55" s="171"/>
+      <c r="O55" s="171"/>
+      <c r="P55" s="171"/>
+      <c r="Q55" s="171"/>
+      <c r="R55" s="171"/>
+      <c r="S55" s="171"/>
+      <c r="T55" s="171"/>
+      <c r="U55" s="171"/>
       <c r="V55" s="114"/>
       <c r="W55" s="114"/>
       <c r="X55" s="114"/>
@@ -6720,7 +6735,7 @@
       <c r="BO55" s="107"/>
       <c r="BP55" s="107"/>
       <c r="BQ55" s="107"/>
-      <c r="BR55" s="138"/>
+      <c r="BR55" s="158"/>
       <c r="BS55" s="39"/>
       <c r="BT55" s="22"/>
       <c r="BU55" s="22"/>
@@ -6732,11 +6747,11 @@
     </row>
     <row r="56" spans="1:78" s="65" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="22"/>
-      <c r="B56" s="135"/>
-      <c r="C56" s="135"/>
-      <c r="D56" s="135"/>
-      <c r="E56" s="135"/>
-      <c r="F56" s="135"/>
+      <c r="B56" s="136"/>
+      <c r="C56" s="136"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="136"/>
+      <c r="F56" s="136"/>
       <c r="G56" s="69" t="s">
         <v>95</v>
       </c>
@@ -6804,7 +6819,7 @@
       <c r="BO56" s="107"/>
       <c r="BP56" s="107"/>
       <c r="BQ56" s="107"/>
-      <c r="BR56" s="138"/>
+      <c r="BR56" s="158"/>
       <c r="BS56" s="39"/>
       <c r="BT56" s="22"/>
       <c r="BU56" s="22"/>
@@ -6816,11 +6831,11 @@
     </row>
     <row r="57" spans="1:78" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="135"/>
-      <c r="C57" s="152"/>
-      <c r="D57" s="152"/>
-      <c r="E57" s="152"/>
-      <c r="F57" s="152"/>
+      <c r="B57" s="136"/>
+      <c r="C57" s="142"/>
+      <c r="D57" s="142"/>
+      <c r="E57" s="142"/>
+      <c r="F57" s="142"/>
       <c r="G57" s="71" t="s">
         <v>96</v>
       </c>
@@ -6888,7 +6903,7 @@
       <c r="BO57" s="43"/>
       <c r="BP57" s="43"/>
       <c r="BQ57" s="43"/>
-      <c r="BR57" s="138"/>
+      <c r="BR57" s="158"/>
       <c r="BS57" s="39"/>
       <c r="BT57" s="22"/>
       <c r="BU57" s="22"/>
@@ -6900,15 +6915,15 @@
     </row>
     <row r="58" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="22"/>
-      <c r="B58" s="153">
+      <c r="B58" s="143">
         <v>3</v>
       </c>
-      <c r="C58" s="154" t="s">
+      <c r="C58" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="135"/>
-      <c r="E58" s="135"/>
-      <c r="F58" s="135"/>
+      <c r="D58" s="136"/>
+      <c r="E58" s="136"/>
+      <c r="F58" s="136"/>
       <c r="G58" s="73" t="s">
         <v>68</v>
       </c>
@@ -6976,7 +6991,7 @@
       <c r="BO58" s="46"/>
       <c r="BP58" s="46"/>
       <c r="BQ58" s="46"/>
-      <c r="BR58" s="138"/>
+      <c r="BR58" s="158"/>
       <c r="BS58" s="22"/>
       <c r="BT58" s="22"/>
       <c r="BU58" s="22"/>
@@ -6988,11 +7003,11 @@
     </row>
     <row r="59" spans="1:78" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="135"/>
-      <c r="C59" s="155"/>
-      <c r="D59" s="155"/>
-      <c r="E59" s="155"/>
-      <c r="F59" s="155"/>
+      <c r="B59" s="136"/>
+      <c r="C59" s="145"/>
+      <c r="D59" s="145"/>
+      <c r="E59" s="145"/>
+      <c r="F59" s="145"/>
       <c r="G59" s="75" t="s">
         <v>96</v>
       </c>
@@ -7060,7 +7075,7 @@
       <c r="BO59" s="53"/>
       <c r="BP59" s="53"/>
       <c r="BQ59" s="53"/>
-      <c r="BR59" s="138"/>
+      <c r="BR59" s="158"/>
       <c r="BS59" s="22"/>
       <c r="BT59" s="22"/>
       <c r="BU59" s="22"/>
@@ -7072,15 +7087,15 @@
     </row>
     <row r="60" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="22"/>
-      <c r="B60" s="145">
+      <c r="B60" s="152">
         <v>4</v>
       </c>
-      <c r="C60" s="156" t="s">
+      <c r="C60" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="D60" s="135"/>
-      <c r="E60" s="135"/>
-      <c r="F60" s="135"/>
+      <c r="D60" s="136"/>
+      <c r="E60" s="136"/>
+      <c r="F60" s="136"/>
       <c r="G60" s="77" t="s">
         <v>67</v>
       </c>
@@ -7148,7 +7163,7 @@
       <c r="BO60" s="46"/>
       <c r="BP60" s="46"/>
       <c r="BQ60" s="46"/>
-      <c r="BR60" s="138"/>
+      <c r="BR60" s="158"/>
       <c r="BS60" s="22"/>
       <c r="BT60" s="22"/>
       <c r="BU60" s="22"/>
@@ -7160,11 +7175,11 @@
     </row>
     <row r="61" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="22"/>
-      <c r="B61" s="135"/>
-      <c r="C61" s="135"/>
-      <c r="D61" s="135"/>
-      <c r="E61" s="135"/>
-      <c r="F61" s="135"/>
+      <c r="B61" s="136"/>
+      <c r="C61" s="136"/>
+      <c r="D61" s="136"/>
+      <c r="E61" s="136"/>
+      <c r="F61" s="136"/>
       <c r="G61" s="77" t="s">
         <v>17</v>
       </c>
@@ -7232,7 +7247,7 @@
       <c r="BO61" s="50"/>
       <c r="BP61" s="50"/>
       <c r="BQ61" s="54"/>
-      <c r="BR61" s="138"/>
+      <c r="BR61" s="158"/>
       <c r="BS61" s="22"/>
       <c r="BT61" s="22"/>
       <c r="BU61" s="22"/>
@@ -7244,11 +7259,11 @@
     </row>
     <row r="62" spans="1:78" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22"/>
-      <c r="B62" s="135"/>
-      <c r="C62" s="157"/>
-      <c r="D62" s="157"/>
-      <c r="E62" s="157"/>
-      <c r="F62" s="157"/>
+      <c r="B62" s="136"/>
+      <c r="C62" s="147"/>
+      <c r="D62" s="147"/>
+      <c r="E62" s="147"/>
+      <c r="F62" s="147"/>
       <c r="G62" s="79" t="s">
         <v>18</v>
       </c>
@@ -7316,7 +7331,7 @@
       <c r="BO62" s="59"/>
       <c r="BP62" s="59"/>
       <c r="BQ62" s="58"/>
-      <c r="BR62" s="138"/>
+      <c r="BR62" s="158"/>
       <c r="BS62" s="22"/>
       <c r="BT62" s="22"/>
       <c r="BU62" s="22"/>
@@ -7328,15 +7343,15 @@
     </row>
     <row r="63" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="22"/>
-      <c r="B63" s="146">
+      <c r="B63" s="135">
         <v>5</v>
       </c>
-      <c r="C63" s="158" t="s">
+      <c r="C63" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="135"/>
-      <c r="E63" s="135"/>
-      <c r="F63" s="135"/>
+      <c r="D63" s="136"/>
+      <c r="E63" s="136"/>
+      <c r="F63" s="136"/>
       <c r="G63" s="81" t="s">
         <v>97</v>
       </c>
@@ -7350,12 +7365,12 @@
       <c r="M63" s="60"/>
       <c r="N63" s="60"/>
       <c r="O63" s="60"/>
-      <c r="P63" s="165"/>
+      <c r="P63" s="130"/>
       <c r="Q63" s="98"/>
       <c r="R63" s="98"/>
       <c r="S63" s="98"/>
       <c r="T63" s="98"/>
-      <c r="U63" s="118"/>
+      <c r="U63" s="170"/>
       <c r="V63" s="96"/>
       <c r="W63" s="96"/>
       <c r="X63" s="96"/>
@@ -7404,7 +7419,7 @@
       <c r="BO63" s="96"/>
       <c r="BP63" s="96"/>
       <c r="BQ63" s="96"/>
-      <c r="BR63" s="138"/>
+      <c r="BR63" s="158"/>
       <c r="BS63" s="22"/>
       <c r="BT63" s="22"/>
       <c r="BU63" s="22"/>
@@ -7416,11 +7431,11 @@
     </row>
     <row r="64" spans="1:78" s="119" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="22"/>
-      <c r="B64" s="146"/>
-      <c r="C64" s="158"/>
-      <c r="D64" s="135"/>
-      <c r="E64" s="135"/>
-      <c r="F64" s="135"/>
+      <c r="B64" s="135"/>
+      <c r="C64" s="148"/>
+      <c r="D64" s="136"/>
+      <c r="E64" s="136"/>
+      <c r="F64" s="136"/>
       <c r="G64" s="81" t="s">
         <v>19</v>
       </c>
@@ -7434,12 +7449,12 @@
       <c r="M64" s="60"/>
       <c r="N64" s="60"/>
       <c r="O64" s="60"/>
-      <c r="P64" s="165"/>
-      <c r="Q64" s="117"/>
-      <c r="R64" s="117"/>
-      <c r="S64" s="117"/>
-      <c r="T64" s="117"/>
-      <c r="U64" s="117"/>
+      <c r="P64" s="130"/>
+      <c r="Q64" s="130"/>
+      <c r="R64" s="130"/>
+      <c r="S64" s="130"/>
+      <c r="T64" s="130"/>
+      <c r="U64" s="130"/>
       <c r="V64" s="87"/>
       <c r="W64" s="87"/>
       <c r="X64" s="87"/>
@@ -7488,7 +7503,7 @@
       <c r="BO64" s="96"/>
       <c r="BP64" s="96"/>
       <c r="BQ64" s="96"/>
-      <c r="BR64" s="138"/>
+      <c r="BR64" s="158"/>
       <c r="BS64" s="22"/>
       <c r="BT64" s="22"/>
       <c r="BU64" s="22"/>
@@ -7500,11 +7515,11 @@
     </row>
     <row r="65" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="22"/>
-      <c r="B65" s="135"/>
-      <c r="C65" s="135"/>
-      <c r="D65" s="135"/>
-      <c r="E65" s="135"/>
-      <c r="F65" s="135"/>
+      <c r="B65" s="136"/>
+      <c r="C65" s="136"/>
+      <c r="D65" s="136"/>
+      <c r="E65" s="136"/>
+      <c r="F65" s="136"/>
       <c r="G65" s="81" t="s">
         <v>20</v>
       </c>
@@ -7556,7 +7571,7 @@
       <c r="AY65" s="96"/>
       <c r="AZ65" s="96"/>
       <c r="BA65" s="98"/>
-      <c r="BB65" s="166"/>
+      <c r="BB65" s="131"/>
       <c r="BC65" s="60"/>
       <c r="BD65" s="60"/>
       <c r="BE65" s="60"/>
@@ -7572,7 +7587,7 @@
       <c r="BO65" s="96"/>
       <c r="BP65" s="96"/>
       <c r="BQ65" s="96"/>
-      <c r="BR65" s="138"/>
+      <c r="BR65" s="158"/>
       <c r="BS65" s="22"/>
       <c r="BT65" s="22"/>
       <c r="BU65" s="22"/>
@@ -7584,11 +7599,11 @@
     </row>
     <row r="66" spans="1:78" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="22"/>
-      <c r="B66" s="135"/>
-      <c r="C66" s="159"/>
-      <c r="D66" s="159"/>
-      <c r="E66" s="159"/>
-      <c r="F66" s="159"/>
+      <c r="B66" s="136"/>
+      <c r="C66" s="149"/>
+      <c r="D66" s="149"/>
+      <c r="E66" s="149"/>
+      <c r="F66" s="149"/>
       <c r="G66" s="83" t="s">
         <v>21</v>
       </c>
@@ -7640,7 +7655,7 @@
       <c r="AY66" s="99"/>
       <c r="AZ66" s="99"/>
       <c r="BA66" s="100"/>
-      <c r="BB66" s="167"/>
+      <c r="BB66" s="132"/>
       <c r="BC66" s="61"/>
       <c r="BD66" s="61"/>
       <c r="BE66" s="61"/>
@@ -7656,7 +7671,7 @@
       <c r="BO66" s="62"/>
       <c r="BP66" s="62"/>
       <c r="BQ66" s="99"/>
-      <c r="BR66" s="138"/>
+      <c r="BR66" s="158"/>
       <c r="BS66" s="22"/>
       <c r="BT66" s="22"/>
       <c r="BU66" s="22"/>
@@ -7828,20 +7843,11 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:F14"/>
-    <mergeCell ref="B15:B57"/>
-    <mergeCell ref="C15:F57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:F59"/>
-    <mergeCell ref="C60:F62"/>
-    <mergeCell ref="C63:F66"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="I2:T2"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="I4:U4"/>
+    <mergeCell ref="X4:AT4"/>
     <mergeCell ref="I5:U5"/>
     <mergeCell ref="I8:Z8"/>
     <mergeCell ref="AA8:AT8"/>
@@ -7852,11 +7858,20 @@
     <mergeCell ref="AA9:AT9"/>
     <mergeCell ref="AU8:BQ8"/>
     <mergeCell ref="AU9:BQ9"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="I2:T2"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="I4:U4"/>
-    <mergeCell ref="X4:AT4"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:F14"/>
+    <mergeCell ref="B15:B57"/>
+    <mergeCell ref="C15:F57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:F59"/>
+    <mergeCell ref="C60:F62"/>
+    <mergeCell ref="C63:F66"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -7886,11 +7901,11 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="164" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">

</xml_diff>